<commit_message>
Added some error checking
</commit_message>
<xml_diff>
--- a/BackEnd/studentsRecords/uploads/genders.xlsx
+++ b/BackEnd/studentsRecords/uploads/genders.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MOCK_DATA (1)" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -353,7 +353,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>